<commit_message>
Included below tests EXL_CorporateLensHomePage_Alerts EXL_CorporateLensHomePage_NewsCarousel EXL_CorporateLensHomePage_Blogs EXL_CorporateLensHomePage_MyDocuments
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/config/Config.xlsx
+++ b/Excelens_Trunk/src/com/proj/config/Config.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Excelens_JWS\Excelens_Trunk_Jul122017\src\com\proj\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT_EXCL_JUL\Excelens_Trunk\src\com\proj\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14865" windowHeight="2820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14865" windowHeight="2820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataFetchFlag" sheetId="1" r:id="rId1"/>
     <sheet name="DataFetchXL" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -178,12 +178,39 @@
   </si>
   <si>
     <t>Alerts</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_NewsCarousel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\src\\com\\proj\\suitecorporateLens\\testdata\\CorporateLensTestData-NewsCarousel.xlsx </t>
+  </si>
+  <si>
+    <t>NewsCarousel</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_Blogs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\src\\com\\proj\\suitecorporateLens\\testdata\\CorporateLensTestData-Blogs.xlsx </t>
+  </si>
+  <si>
+    <t>Blogs</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_MyDocuments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\src\\com\\proj\\suitecorporateLens\\testdata\\CorporateLensTestData-MyDocuments.xlsx </t>
+  </si>
+  <si>
+    <t>NewDocument</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -598,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -746,9 +773,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B20">
       <formula1>"XL,DB"</formula1>
     </dataValidation>
   </dataValidations>
@@ -760,10 +811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -958,6 +1009,39 @@
       </c>
       <c r="C17" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -978,10 +1062,13 @@
     <hyperlink ref="B15" r:id="rId14"/>
     <hyperlink ref="B16" r:id="rId15"/>
     <hyperlink ref="B17" r:id="rId16"/>
+    <hyperlink ref="B18" r:id="rId17"/>
+    <hyperlink ref="B19" r:id="rId18"/>
+    <hyperlink ref="B20" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId17"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New Test :- EXL_CorporateLensHomePage_MyFavourites
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/config/Config.xlsx
+++ b/Excelens_Trunk/src/com/proj/config/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14865" windowHeight="2820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14865" windowHeight="2820"/>
   </bookViews>
   <sheets>
     <sheet name="DataFetchFlag" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>NewDocument</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_MyFavourites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\src\\com\\proj\\suitecorporateLens\\testdata\\CorporateLensTestData-MyFavourites.xlsx </t>
+  </si>
+  <si>
+    <t>Favourites</t>
   </si>
 </sst>
 </file>
@@ -625,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -797,9 +806,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B21">
       <formula1>"XL,DB"</formula1>
     </dataValidation>
   </dataValidations>
@@ -811,10 +828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1042,6 +1059,17 @@
       </c>
       <c r="C20" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1065,10 +1093,11 @@
     <hyperlink ref="B18" r:id="rId17"/>
     <hyperlink ref="B19" r:id="rId18"/>
     <hyperlink ref="B20" r:id="rId19"/>
+    <hyperlink ref="B21" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId20"/>
+  <legacyDrawing r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Included new test - EXL_CorporateLensHomePage_Announcements
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/config/Config.xlsx
+++ b/Excelens_Trunk/src/com/proj/config/Config.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -214,6 +214,15 @@
   </si>
   <si>
     <t>Favourites</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_Announcements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\src\\com\\proj\\suitecorporateLens\\testdata\\CorporateLensTestData-Announcements.xlsx </t>
+  </si>
+  <si>
+    <t>Announcements</t>
   </si>
 </sst>
 </file>
@@ -634,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -814,9 +823,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B22">
       <formula1>"XL,DB"</formula1>
     </dataValidation>
   </dataValidations>
@@ -828,10 +845,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1070,6 +1087,17 @@
       </c>
       <c r="C21" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1094,10 +1122,11 @@
     <hyperlink ref="B19" r:id="rId18"/>
     <hyperlink ref="B20" r:id="rId19"/>
     <hyperlink ref="B21" r:id="rId20"/>
+    <hyperlink ref="B22" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId21"/>
+  <legacyDrawing r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Included new test EXL_CorporateLensHomePage_CalendarEvent
</commit_message>
<xml_diff>
--- a/Excelens_Trunk/src/com/proj/config/Config.xlsx
+++ b/Excelens_Trunk/src/com/proj/config/Config.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>Announcements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\src\\com\\proj\\suitecorporateLens\\testdata\\CorporateLensTestData-Calendar.xlsx </t>
+  </si>
+  <si>
+    <t>New Event</t>
+  </si>
+  <si>
+    <t>EXL_CorporateLensHomePage_CalendarEvent</t>
   </si>
 </sst>
 </file>
@@ -643,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -831,9 +840,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B23">
       <formula1>"XL,DB"</formula1>
     </dataValidation>
   </dataValidations>
@@ -845,10 +862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1098,6 +1115,17 @@
       </c>
       <c r="C22" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1123,10 +1151,11 @@
     <hyperlink ref="B20" r:id="rId19"/>
     <hyperlink ref="B21" r:id="rId20"/>
     <hyperlink ref="B22" r:id="rId21"/>
+    <hyperlink ref="B23" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId22"/>
+  <legacyDrawing r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>